<commit_message>
result step 3 and 4
</commit_message>
<xml_diff>
--- a/3.results/model_selection/mouette_melanocephale_HR_3_blocks_assemblage.xlsx
+++ b/3.results/model_selection/mouette_melanocephale_HR_3_blocks_assemblage.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schroll\Documents\stage_M2\3.results\model_selection\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\louis\OneDrive\Documents\stage_M2\3.results\model_selection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{581DFE32-81A5-4E02-ACE5-C556F733918C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{817CAF06-1DED-406A-933F-6D34C1A5ED90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-107" yWindow="-107" windowWidth="20847" windowHeight="11111" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="blocks" sheetId="1" r:id="rId1"/>
@@ -180,7 +180,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="9">
     <dxf>
       <font>
         <b/>
@@ -244,66 +244,6 @@
         <color rgb="FFFFB6C1"/>
         <name val="Calibri"/>
       </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF006400"/>
-        <name val="Calibri"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF90EE90"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF006400"/>
-        <name val="Calibri"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF90EE90"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF006400"/>
-        <name val="Calibri"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF90EE90"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF006400"/>
-        <name val="Calibri"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF90EE90"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="11"/>
-        <color rgb="FF006400"/>
-        <name val="Calibri"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF90EE90"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -615,9 +555,9 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -700,42 +640,42 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B2" s="1">
-        <v>1.2969999999999999</v>
+        <v>1.0249999999999999</v>
       </c>
       <c r="C2" s="1">
-        <v>104.3</v>
+        <v>130.6</v>
       </c>
       <c r="D2" s="1">
-        <v>0.63</v>
+        <v>0.64</v>
       </c>
       <c r="E2" s="1">
-        <v>0.51</v>
+        <v>0.5</v>
       </c>
       <c r="F2" s="1">
         <v>0.42</v>
       </c>
       <c r="G2" s="1">
-        <v>0.51</v>
+        <v>0.5</v>
       </c>
       <c r="H2" s="1">
-        <v>0.43</v>
+        <v>0.44</v>
       </c>
       <c r="I2" s="1">
-        <v>0.49</v>
+        <v>0.5</v>
       </c>
       <c r="J2" s="1">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="K2" s="1">
         <v>147</v>
       </c>
       <c r="L2" s="1">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="M2" s="1">
         <v>1178</v>
@@ -747,62 +687,62 @@
         <v>147</v>
       </c>
       <c r="P2" s="1">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="Q2" s="1">
-        <v>1172</v>
+        <v>1173</v>
       </c>
       <c r="R2" s="1">
-        <v>-1.7</v>
+        <v>-1.6</v>
       </c>
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
       <c r="U2" s="1"/>
       <c r="V2" s="1"/>
       <c r="W2" s="1">
-        <v>0.45</v>
+        <v>0.39</v>
       </c>
       <c r="X2" s="1"/>
       <c r="Y2" s="1"/>
       <c r="Z2" s="1"/>
       <c r="AA2" s="1"/>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B3" s="1">
-        <v>1.0189999999999999</v>
+        <v>1.0129999999999999</v>
       </c>
       <c r="C3" s="1">
-        <v>119.9</v>
+        <v>126.3</v>
       </c>
       <c r="D3" s="1">
-        <v>0.65</v>
+        <v>0.63</v>
       </c>
       <c r="E3" s="1">
+        <v>0.49</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0.41</v>
+      </c>
+      <c r="G3" s="1">
         <v>0.51</v>
       </c>
-      <c r="F3" s="1">
-        <v>0.42</v>
-      </c>
-      <c r="G3" s="1">
-        <v>0.5</v>
-      </c>
       <c r="H3" s="1">
-        <v>0.44</v>
+        <v>0.45</v>
       </c>
       <c r="I3" s="1">
         <v>0.5</v>
       </c>
       <c r="J3" s="1">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="K3" s="1">
         <v>149</v>
       </c>
       <c r="L3" s="1">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="M3" s="1">
         <v>1184</v>
@@ -814,48 +754,52 @@
         <v>149</v>
       </c>
       <c r="P3" s="1">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="Q3" s="1">
-        <v>1181</v>
-      </c>
-      <c r="R3" s="1"/>
+        <v>1182</v>
+      </c>
+      <c r="R3" s="1">
+        <v>-1.4</v>
+      </c>
       <c r="S3" s="1"/>
       <c r="T3" s="1">
-        <v>2.99</v>
+        <v>1.46</v>
       </c>
       <c r="U3" s="1"/>
       <c r="V3" s="1">
-        <v>-0.94</v>
-      </c>
-      <c r="W3" s="1"/>
+        <v>-0.43</v>
+      </c>
+      <c r="W3" s="1">
+        <v>0.5</v>
+      </c>
       <c r="X3" s="1"/>
       <c r="Y3" s="1">
-        <v>0.92</v>
+        <v>1.24</v>
       </c>
       <c r="Z3" s="1"/>
       <c r="AA3" s="1">
-        <v>0.46</v>
+        <v>0.66</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B4" s="1">
-        <v>1.0109999999999999</v>
+        <v>1.022</v>
       </c>
       <c r="C4" s="1">
-        <v>190.1</v>
+        <v>177</v>
       </c>
       <c r="D4" s="1">
-        <v>0.63</v>
+        <v>0.62</v>
       </c>
       <c r="E4" s="1">
-        <v>0.51</v>
+        <v>0.5</v>
       </c>
       <c r="F4" s="1">
-        <v>0.41</v>
+        <v>0.4</v>
       </c>
       <c r="G4" s="1">
         <v>0.51</v>
@@ -885,54 +829,66 @@
         <v>147</v>
       </c>
       <c r="P4" s="1">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="Q4" s="1">
-        <v>1176</v>
-      </c>
-      <c r="R4" s="1"/>
+        <v>1177</v>
+      </c>
+      <c r="R4" s="1">
+        <v>-0.96</v>
+      </c>
       <c r="S4" s="1">
-        <v>2.0499999999999998</v>
-      </c>
-      <c r="T4" s="1"/>
+        <v>0.65</v>
+      </c>
+      <c r="T4" s="1">
+        <v>1.51</v>
+      </c>
       <c r="U4" s="1">
-        <v>-3.4</v>
-      </c>
-      <c r="V4" s="1"/>
-      <c r="W4" s="1"/>
+        <v>-1.53</v>
+      </c>
+      <c r="V4" s="1">
+        <v>-0.53</v>
+      </c>
+      <c r="W4" s="1">
+        <v>0.48</v>
+      </c>
       <c r="X4" s="1">
-        <v>0.66</v>
-      </c>
-      <c r="Y4" s="1"/>
+        <v>0.96</v>
+      </c>
+      <c r="Y4" s="1">
+        <v>1.18</v>
+      </c>
       <c r="Z4" s="1">
-        <v>0.77</v>
-      </c>
-      <c r="AA4" s="1"/>
+        <v>0.96</v>
+      </c>
+      <c r="AA4" s="1">
+        <v>0.64</v>
+      </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B5" s="1">
-        <v>1.097</v>
+        <v>1.119</v>
       </c>
       <c r="C5" s="1">
-        <v>82</v>
+        <v>79.599999999999994</v>
       </c>
       <c r="D5" s="1">
         <v>0.63</v>
       </c>
       <c r="E5" s="1">
-        <v>0.51</v>
+        <v>0.5</v>
       </c>
       <c r="F5" s="1">
-        <v>0.41</v>
+        <v>0.42</v>
       </c>
       <c r="G5" s="1">
         <v>0.5</v>
       </c>
       <c r="H5" s="1">
-        <v>0.44</v>
+        <v>0.43</v>
       </c>
       <c r="I5" s="1">
         <v>0.5</v>
@@ -962,46 +918,46 @@
         <v>1175</v>
       </c>
       <c r="R5" s="1">
-        <v>-1.33</v>
-      </c>
-      <c r="S5" s="1"/>
-      <c r="T5" s="1">
-        <v>1.41</v>
-      </c>
-      <c r="U5" s="1"/>
-      <c r="V5" s="1">
-        <v>-0.35</v>
-      </c>
+        <v>-1.22</v>
+      </c>
+      <c r="S5" s="1">
+        <v>0.62</v>
+      </c>
+      <c r="T5" s="1"/>
+      <c r="U5" s="1">
+        <v>-1.56</v>
+      </c>
+      <c r="V5" s="1"/>
       <c r="W5" s="1">
-        <v>0.48</v>
-      </c>
-      <c r="X5" s="1"/>
-      <c r="Y5" s="1">
-        <v>1.2</v>
-      </c>
-      <c r="Z5" s="1"/>
-      <c r="AA5" s="1">
-        <v>0.64</v>
-      </c>
+        <v>0.45</v>
+      </c>
+      <c r="X5" s="1">
+        <v>0.94</v>
+      </c>
+      <c r="Y5" s="1"/>
+      <c r="Z5" s="1">
+        <v>1.01</v>
+      </c>
+      <c r="AA5" s="1"/>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B6" s="1">
-        <v>1.093</v>
+        <v>1.008</v>
       </c>
       <c r="C6" s="1">
-        <v>124.7</v>
+        <v>146.6</v>
       </c>
       <c r="D6" s="1">
-        <v>0.63</v>
+        <v>0.62</v>
       </c>
       <c r="E6" s="1">
-        <v>0.51</v>
+        <v>0.5</v>
       </c>
       <c r="F6" s="1">
-        <v>0.4</v>
+        <v>0.41</v>
       </c>
       <c r="G6" s="1">
         <v>0.5</v>
@@ -1016,19 +972,19 @@
         <v>635</v>
       </c>
       <c r="K6" s="1">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="L6" s="1">
         <v>394</v>
       </c>
       <c r="M6" s="1">
-        <v>1175</v>
+        <v>1176</v>
       </c>
       <c r="N6" s="1">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="O6" s="1">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="P6" s="1">
         <v>394</v>
@@ -1036,62 +992,58 @@
       <c r="Q6" s="1">
         <v>1169</v>
       </c>
-      <c r="R6" s="1">
-        <v>-1.23</v>
-      </c>
-      <c r="S6" s="1">
-        <v>0.65</v>
-      </c>
-      <c r="T6" s="1"/>
-      <c r="U6" s="1">
-        <v>-1.56</v>
-      </c>
-      <c r="V6" s="1"/>
-      <c r="W6" s="1">
+      <c r="R6" s="1"/>
+      <c r="S6" s="1"/>
+      <c r="T6" s="1">
+        <v>2.95</v>
+      </c>
+      <c r="U6" s="1"/>
+      <c r="V6" s="1">
+        <v>-0.93</v>
+      </c>
+      <c r="W6" s="1"/>
+      <c r="X6" s="1"/>
+      <c r="Y6" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="Z6" s="1"/>
+      <c r="AA6" s="1">
         <v>0.47</v>
       </c>
-      <c r="X6" s="1">
-        <v>0.94</v>
-      </c>
-      <c r="Y6" s="1"/>
-      <c r="Z6" s="1">
-        <v>0.99</v>
-      </c>
-      <c r="AA6" s="1"/>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B7" s="1">
-        <v>1.0289999999999999</v>
+        <v>1.0880000000000001</v>
       </c>
       <c r="C7" s="1">
-        <v>81.2</v>
+        <v>81.900000000000006</v>
       </c>
       <c r="D7" s="1">
-        <v>0.62</v>
+        <v>0.61</v>
       </c>
       <c r="E7" s="1">
-        <v>0.5</v>
+        <v>0.49</v>
       </c>
       <c r="F7" s="1">
         <v>0.4</v>
       </c>
       <c r="G7" s="1">
-        <v>0.5</v>
+        <v>0.51</v>
       </c>
       <c r="H7" s="1">
         <v>0.48</v>
       </c>
       <c r="I7" s="1">
-        <v>0.52</v>
+        <v>0.51</v>
       </c>
       <c r="J7" s="1">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="K7" s="1">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="L7" s="1">
         <v>394</v>
@@ -1100,7 +1052,7 @@
         <v>1173</v>
       </c>
       <c r="N7" s="1">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="O7" s="1">
         <v>147</v>
@@ -1109,50 +1061,50 @@
         <v>396</v>
       </c>
       <c r="Q7" s="1">
-        <v>1170</v>
+        <v>1169</v>
       </c>
       <c r="R7" s="1"/>
       <c r="S7" s="1">
-        <v>1.39</v>
+        <v>1.44</v>
       </c>
       <c r="T7" s="1">
-        <v>2.39</v>
+        <v>2.31</v>
       </c>
       <c r="U7" s="1">
-        <v>-2.48</v>
+        <v>-2.4500000000000002</v>
       </c>
       <c r="V7" s="1">
-        <v>-0.86</v>
+        <v>-0.8</v>
       </c>
       <c r="W7" s="1"/>
       <c r="X7" s="1">
-        <v>0.81</v>
+        <v>0.79</v>
       </c>
       <c r="Y7" s="1">
-        <v>1.07</v>
+        <v>1.05</v>
       </c>
       <c r="Z7" s="1">
-        <v>0.81</v>
+        <v>0.82</v>
       </c>
       <c r="AA7" s="1">
-        <v>0.57999999999999996</v>
+        <v>0.56999999999999995</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B8" s="1">
-        <v>1.099</v>
+        <v>1.0289999999999999</v>
       </c>
       <c r="C8" s="1">
-        <v>67.599999999999994</v>
+        <v>95.5</v>
       </c>
       <c r="D8" s="1">
         <v>0.61</v>
       </c>
       <c r="E8" s="1">
-        <v>0.49</v>
+        <v>0.5</v>
       </c>
       <c r="F8" s="1">
         <v>0.41</v>
@@ -1161,7 +1113,7 @@
         <v>0.5</v>
       </c>
       <c r="H8" s="1">
-        <v>0.47</v>
+        <v>0.46</v>
       </c>
       <c r="I8" s="1">
         <v>0.5</v>
@@ -1173,92 +1125,53 @@
         <v>147</v>
       </c>
       <c r="L8" s="1">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="M8" s="1">
-        <v>1176</v>
+        <v>1174</v>
       </c>
       <c r="N8" s="1">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="O8" s="1">
         <v>146</v>
       </c>
       <c r="P8" s="1">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="Q8" s="1">
         <v>1170</v>
       </c>
-      <c r="R8" s="1">
-        <v>-1</v>
-      </c>
+      <c r="R8" s="1"/>
       <c r="S8" s="1">
-        <v>0.74</v>
-      </c>
-      <c r="T8" s="1">
-        <v>1.1499999999999999</v>
-      </c>
+        <v>2.0699999999999998</v>
+      </c>
+      <c r="T8" s="1"/>
       <c r="U8" s="1">
-        <v>-1.55</v>
-      </c>
-      <c r="V8" s="1">
-        <v>-0.37</v>
-      </c>
-      <c r="W8" s="1">
-        <v>0.52</v>
-      </c>
+        <v>-3.43</v>
+      </c>
+      <c r="V8" s="1"/>
+      <c r="W8" s="1"/>
       <c r="X8" s="1">
-        <v>0.98</v>
-      </c>
-      <c r="Y8" s="1">
-        <v>1.25</v>
-      </c>
+        <v>0.65</v>
+      </c>
+      <c r="Y8" s="1"/>
       <c r="Z8" s="1">
-        <v>0.99</v>
-      </c>
-      <c r="AA8" s="1">
-        <v>0.67</v>
-      </c>
+        <v>0.79</v>
+      </c>
+      <c r="AA8" s="1"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D8">
-    <cfRule type="cellIs" dxfId="13" priority="22" operator="between">
-      <formula>0.1</formula>
-      <formula>0.9</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E8">
-    <cfRule type="cellIs" dxfId="12" priority="21" operator="between">
-      <formula>0.1</formula>
-      <formula>0.9</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F8">
-    <cfRule type="cellIs" dxfId="11" priority="20" operator="between">
-      <formula>0.1</formula>
-      <formula>0.9</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G8">
-    <cfRule type="cellIs" dxfId="10" priority="19" operator="between">
-      <formula>0.1</formula>
-      <formula>0.9</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H8">
-    <cfRule type="cellIs" dxfId="9" priority="18" operator="between">
-      <formula>0.1</formula>
-      <formula>0.9</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I8">
+  <conditionalFormatting sqref="D2:I8">
     <cfRule type="cellIs" dxfId="8" priority="17" operator="between">
       <formula>0.1</formula>
       <formula>0.9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:J8">
+    <cfRule type="expression" dxfId="7" priority="15">
+      <formula>J2&lt;625</formula>
+    </cfRule>
     <cfRule type="colorScale" priority="16">
       <colorScale>
         <cfvo type="min"/>
@@ -1267,11 +1180,11 @@
         <color rgb="FFFFFFFF"/>
       </colorScale>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="15">
-      <formula>J2&lt;628</formula>
-    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K8">
+    <cfRule type="expression" dxfId="6" priority="13">
+      <formula>K2&lt;150</formula>
+    </cfRule>
     <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="min"/>
@@ -1280,11 +1193,11 @@
         <color rgb="FFFFFFFF"/>
       </colorScale>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="13">
-      <formula>K2&lt;151</formula>
-    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2:L8">
+    <cfRule type="expression" dxfId="5" priority="11">
+      <formula>L2&lt;396</formula>
+    </cfRule>
     <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="min"/>
@@ -1293,11 +1206,11 @@
         <color rgb="FFFFFFFF"/>
       </colorScale>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="11">
-      <formula>L2&lt;399</formula>
-    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:M8">
+    <cfRule type="expression" dxfId="4" priority="9">
+      <formula>M2&lt;1176</formula>
+    </cfRule>
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min"/>
@@ -1306,11 +1219,11 @@
         <color rgb="FFFFFFFF"/>
       </colorScale>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="9">
-      <formula>M2&lt;1178</formula>
-    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2:N8">
+    <cfRule type="expression" dxfId="3" priority="7">
+      <formula>N2&lt;622</formula>
+    </cfRule>
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
@@ -1319,11 +1232,11 @@
         <color rgb="FFFFFFFF"/>
       </colorScale>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="7">
-      <formula>N2&lt;624</formula>
-    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O2:O8">
+    <cfRule type="expression" dxfId="2" priority="5">
+      <formula>O2&lt;149</formula>
+    </cfRule>
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
@@ -1332,11 +1245,11 @@
         <color rgb="FFFFFFFF"/>
       </colorScale>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="5">
-      <formula>O2&lt;151</formula>
-    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P2:P8">
+    <cfRule type="expression" dxfId="1" priority="3">
+      <formula>P2&lt;397</formula>
+    </cfRule>
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -1345,11 +1258,11 @@
         <color rgb="FFFFFFFF"/>
       </colorScale>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="3">
-      <formula>P2&lt;399</formula>
-    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q2:Q8">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>Q2&lt;1172</formula>
+    </cfRule>
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -1358,9 +1271,6 @@
         <color rgb="FFFFFFFF"/>
       </colorScale>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="1">
-      <formula>Q2&lt;1174</formula>
-    </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>